<commit_message>
fix: new competitions has now listeners, table view and create button relationship
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -7,14 +7,16 @@
   </bookViews>
   <sheets>
     <sheet name="Name" r:id="rId3" sheetId="1"/>
-    <sheet name="CyberuHub" r:id="rId4" sheetId="2"/>
-    <sheet name="AIoT Hackathon with stc" r:id="rId5" sheetId="3"/>
+    <sheet name="hakathon" r:id="rId4" sheetId="2"/>
+    <sheet name="CTF" r:id="rId5" sheetId="3"/>
+    <sheet name="CyberuHub" r:id="rId6" sheetId="4"/>
+    <sheet name="new challange" r:id="rId7" sheetId="5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
   <si>
     <t>Competition</t>
   </si>
@@ -43,6 +45,21 @@
     <t>Rank</t>
   </si>
   <si>
+    <t>hakathon</t>
+  </si>
+  <si>
+    <t>www.google.com</t>
+  </si>
+  <si>
+    <t>CTF</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>Team Name</t>
+  </si>
+  <si>
     <t>CyberuHub</t>
   </si>
   <si>
@@ -97,55 +114,7 @@
     <t>SWE</t>
   </si>
   <si>
-    <t>AIoT Hackathon with stc</t>
-  </si>
-  <si>
-    <t>https://ultrahack.org/aiot-hackathon-stc</t>
-  </si>
-  <si>
-    <t>team</t>
-  </si>
-  <si>
-    <t>Team Name</t>
-  </si>
-  <si>
-    <t>SuperDevops</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>222243860</t>
-  </si>
-  <si>
-    <t>Bassel Alqahtani</t>
-  </si>
-  <si>
-    <t>222246560</t>
-  </si>
-  <si>
-    <t>Naif Essam</t>
-  </si>
-  <si>
-    <t>StackUnderflow</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>222219260</t>
-  </si>
-  <si>
-    <t>Majed Ahmad</t>
-  </si>
-  <si>
-    <t>COE</t>
-  </si>
-  <si>
-    <t>222267500</t>
-  </si>
-  <si>
-    <t>Saleh Mohammed</t>
+    <t>new challange</t>
   </si>
 </sst>
 </file>
@@ -272,6 +241,132 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="12.01953125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="16.30859375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.53515625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="6.0703125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="5.42578125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>36872.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s" s="1">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s" s="1">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="12.01953125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="16.30859375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.53515625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="6.0703125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="5.4765625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.62890625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="5.42578125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>36880.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s" s="1">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s" s="1">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s" s="1">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s" s="1">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -290,7 +385,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -298,7 +393,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -306,7 +401,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>44471.0</v>
+        <v>44836.0</v>
       </c>
     </row>
     <row r="5">
@@ -329,16 +424,16 @@
         <v>1.0</v>
       </c>
       <c r="B6" t="s" s="1">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s" s="1">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -346,16 +441,16 @@
         <v>2.0</v>
       </c>
       <c r="B7" t="s" s="1">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s" s="1">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s" s="1">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s" s="1">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
@@ -363,16 +458,16 @@
         <v>3.0</v>
       </c>
       <c r="B8" t="s" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s" s="1">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s" s="1">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s" s="1">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
@@ -380,16 +475,16 @@
         <v>4.0</v>
       </c>
       <c r="B9" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s" s="1">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s" s="1">
         <v>24</v>
-      </c>
-      <c r="C9" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s" s="1">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s" s="1">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -397,20 +492,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="12.01953125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="38.27734375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="16.765625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="16.30859375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.53515625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="6.0703125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="5.4765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="14.81640625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.62890625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="5.42578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -419,7 +514,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
@@ -427,7 +522,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -435,7 +530,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>44481.0</v>
+        <v>44897.0</v>
       </c>
     </row>
     <row r="5">
@@ -450,105 +545,13 @@
         <v>7</v>
       </c>
       <c r="E5" t="s" s="1">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s" s="1">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s" s="1">
         <v>8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B6" t="s" s="1">
-        <v>33</v>
-      </c>
-      <c r="C6" t="s" s="1">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s" s="1">
-        <v>14</v>
-      </c>
-      <c r="E6" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="F6" t="s" s="1">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="B7" t="s" s="1">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s" s="1">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s" s="1">
-        <v>26</v>
-      </c>
-      <c r="E7" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="F7" t="s" s="1">
-        <v>31</v>
-      </c>
-      <c r="G7" t="s" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B8" t="s" s="1">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s" s="1">
-        <v>40</v>
-      </c>
-      <c r="D8" t="s" s="1">
-        <v>41</v>
-      </c>
-      <c r="E8" t="n" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="F8" t="s" s="1">
-        <v>37</v>
-      </c>
-      <c r="G8" t="s" s="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="B9" t="s" s="1">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s" s="1">
-        <v>43</v>
-      </c>
-      <c r="D9" t="s" s="1">
-        <v>41</v>
-      </c>
-      <c r="E9" t="n" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="F9" t="s" s="1">
-        <v>37</v>
-      </c>
-      <c r="G9" t="s" s="1">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>